<commit_message>
First full version of diag_ss.bib
</commit_message>
<xml_diff>
--- a/scripts/script_data/complete_MANUAL_LOOKUP_matches_single_bibkey_with_many_ss_ids_KM.xlsx
+++ b/scripts/script_data/complete_MANUAL_LOOKUP_matches_single_bibkey_with_many_ss_ids_KM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="232">
   <si>
     <t>bibkey</t>
   </si>
@@ -710,9 +710,6 @@
   </si>
   <si>
     <t>title matching: single bibkey with multiple_ss_ids (['ebb0d21c567909e31be5d43d72c8b3020f2708c9', 'fd2239f855b044b6ebe9fac5e0e01951bc9eddb4']), took the first one with most citations</t>
-  </si>
-  <si>
-    <t>BOLD means not checked yet! (same doi…. Do I need to?) --&gt; JOEY: I made them all True for adding, and all false for blacklist</t>
   </si>
 </sst>
 </file>
@@ -725,7 +722,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,13 +748,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1225,148 +1215,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1733,7 +1723,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2960,9 +2950,7 @@
       </c>
     </row>
     <row r="36" spans="9:9">
-      <c r="I36" s="2" t="s">
-        <v>232</v>
-      </c>
+      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="9:9">
       <c r="I37" s="6"/>

</xml_diff>